<commit_message>
minor changes, parameter updates, new data sources
</commit_message>
<xml_diff>
--- a/Misc/HampsonTable.xlsx
+++ b/Misc/HampsonTable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronanderson/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronanderson/Desktop/BioEcon_CanineRabies/Misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,11 +13,12 @@
   </bookViews>
   <sheets>
     <sheet name="Table S1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table S1'!$A$7:$BC$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table S1'!$A$7:$BC$199</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000" iterate="1" iterateCount="50" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1990" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2056" uniqueCount="474">
   <si>
     <t>TD = time discounting (0.03), AW = age-weighting (C = 0.1658, Beta = 0.04)</t>
   </si>
@@ -1489,6 +1490,15 @@
   </si>
   <si>
     <t>Rabies burden model</t>
+  </si>
+  <si>
+    <t>total bites</t>
+  </si>
+  <si>
+    <t>total rabid bites</t>
+  </si>
+  <si>
+    <t>total non-rabid bites</t>
   </si>
 </sst>
 </file>
@@ -1654,7 +1664,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1718,6 +1728,12 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2056,19 +2072,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:BC199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="7" topLeftCell="F31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="7" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M7" sqref="M7"/>
+      <selection pane="bottomRight" activeCell="L203" sqref="L203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
     <col min="8" max="8" width="12.1640625" customWidth="1"/>
@@ -2584,7 +2602,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2751,7 +2769,7 @@
         <v>473894.47456714901</v>
       </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2918,7 +2936,7 @@
         <v>1193473.8129525499</v>
       </c>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -3252,7 +3270,7 @@
         <v>552817.29261443904</v>
       </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>5</v>
       </c>
@@ -3419,7 +3437,7 @@
         <v>1963354.7921497801</v>
       </c>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>6</v>
       </c>
@@ -3586,7 +3604,7 @@
         <v>198913.87982612901</v>
       </c>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>7</v>
       </c>
@@ -3753,7 +3771,7 @@
         <v>1230506.9898138901</v>
       </c>
     </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>8</v>
       </c>
@@ -3920,7 +3938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>9</v>
       </c>
@@ -4087,7 +4105,7 @@
         <v>1041639.1051498899</v>
       </c>
     </row>
-    <row r="17" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>10</v>
       </c>
@@ -4421,7 +4439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>12</v>
       </c>
@@ -4588,7 +4606,7 @@
         <v>46159.727977258597</v>
       </c>
     </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>13</v>
       </c>
@@ -4755,7 +4773,7 @@
         <v>281055.64034275</v>
       </c>
     </row>
-    <row r="21" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>14</v>
       </c>
@@ -4922,7 +4940,7 @@
         <v>386734.35997843702</v>
       </c>
     </row>
-    <row r="22" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>15</v>
       </c>
@@ -5089,7 +5107,7 @@
         <v>117584.868147799</v>
       </c>
     </row>
-    <row r="23" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>16</v>
       </c>
@@ -5256,7 +5274,7 @@
         <v>591298.03454115801</v>
       </c>
     </row>
-    <row r="24" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>17</v>
       </c>
@@ -5423,7 +5441,7 @@
         <v>3135.14060001494</v>
       </c>
     </row>
-    <row r="25" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>18</v>
       </c>
@@ -5757,7 +5775,7 @@
         <v>10523445.6443983</v>
       </c>
     </row>
-    <row r="27" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>20</v>
       </c>
@@ -5924,7 +5942,7 @@
         <v>20179.204842749699</v>
       </c>
     </row>
-    <row r="28" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>21</v>
       </c>
@@ -6091,7 +6109,7 @@
         <v>84787.324258291497</v>
       </c>
     </row>
-    <row r="29" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>22</v>
       </c>
@@ -6258,7 +6276,7 @@
         <v>419509.73757909797</v>
       </c>
     </row>
-    <row r="30" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>23</v>
       </c>
@@ -6425,7 +6443,7 @@
         <v>1218365.0118438499</v>
       </c>
     </row>
-    <row r="31" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>24</v>
       </c>
@@ -6926,7 +6944,7 @@
         <v>191571.784770114</v>
       </c>
     </row>
-    <row r="34" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>27</v>
       </c>
@@ -7093,7 +7111,7 @@
         <v>18578.694578875198</v>
       </c>
     </row>
-    <row r="35" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>28</v>
       </c>
@@ -7594,7 +7612,7 @@
         <v>261039.07839816299</v>
       </c>
     </row>
-    <row r="38" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>31</v>
       </c>
@@ -7761,7 +7779,7 @@
         <v>1800204.7627971401</v>
       </c>
     </row>
-    <row r="39" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>32</v>
       </c>
@@ -8095,7 +8113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>34</v>
       </c>
@@ -8596,7 +8614,7 @@
         <v>643890.02602521202</v>
       </c>
     </row>
-    <row r="44" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>37</v>
       </c>
@@ -8763,7 +8781,7 @@
         <v>1953658.7647514199</v>
       </c>
     </row>
-    <row r="45" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>38</v>
       </c>
@@ -8930,7 +8948,7 @@
         <v>3005093.11793959</v>
       </c>
     </row>
-    <row r="46" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>39</v>
       </c>
@@ -9097,7 +9115,7 @@
         <v>105230.208519362</v>
       </c>
     </row>
-    <row r="47" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>40</v>
       </c>
@@ -9264,7 +9282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>41</v>
       </c>
@@ -9598,7 +9616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>43</v>
       </c>
@@ -9765,7 +9783,7 @@
         <v>84811.836349721896</v>
       </c>
     </row>
-    <row r="51" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>44</v>
       </c>
@@ -10099,7 +10117,7 @@
         <v>77310.888517116298</v>
       </c>
     </row>
-    <row r="53" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>46</v>
       </c>
@@ -10433,7 +10451,7 @@
         <v>127588.838940762</v>
       </c>
     </row>
-    <row r="55" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>48</v>
       </c>
@@ -10600,7 +10618,7 @@
         <v>107074.980465172</v>
       </c>
     </row>
-    <row r="56" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>49</v>
       </c>
@@ -11435,7 +11453,7 @@
         <v>770574.11437385797</v>
       </c>
     </row>
-    <row r="61" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>54</v>
       </c>
@@ -11602,7 +11620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>55</v>
       </c>
@@ -11769,7 +11787,7 @@
         <v>5798398.8867808804</v>
       </c>
     </row>
-    <row r="63" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>56</v>
       </c>
@@ -11936,7 +11954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>57</v>
       </c>
@@ -12103,7 +12121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>58</v>
       </c>
@@ -12270,7 +12288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>59</v>
       </c>
@@ -12437,7 +12455,7 @@
         <v>7199.7334316959495</v>
       </c>
     </row>
-    <row r="67" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>60</v>
       </c>
@@ -12604,7 +12622,7 @@
         <v>568695.02222116396</v>
       </c>
     </row>
-    <row r="68" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>61</v>
       </c>
@@ -12771,7 +12789,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>62</v>
       </c>
@@ -12938,7 +12956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>63</v>
       </c>
@@ -13105,7 +13123,7 @@
         <v>42346.853422732704</v>
       </c>
     </row>
-    <row r="71" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>64</v>
       </c>
@@ -13272,7 +13290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>65</v>
       </c>
@@ -13439,7 +13457,7 @@
         <v>19872.132600541201</v>
       </c>
     </row>
-    <row r="73" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>66</v>
       </c>
@@ -13606,7 +13624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>67</v>
       </c>
@@ -13773,7 +13791,7 @@
         <v>215851.120557571</v>
       </c>
     </row>
-    <row r="75" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>68</v>
       </c>
@@ -13940,7 +13958,7 @@
         <v>3198.0105071084499</v>
       </c>
     </row>
-    <row r="76" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>69</v>
       </c>
@@ -14107,7 +14125,7 @@
         <v>4692.5560366672398</v>
       </c>
     </row>
-    <row r="77" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>70</v>
       </c>
@@ -14274,7 +14292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>71</v>
       </c>
@@ -14441,7 +14459,7 @@
         <v>15248.261840556401</v>
       </c>
     </row>
-    <row r="79" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>72</v>
       </c>
@@ -14608,7 +14626,7 @@
         <v>364.33091288921003</v>
       </c>
     </row>
-    <row r="80" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>73</v>
       </c>
@@ -14775,7 +14793,7 @@
         <v>107514.565510628</v>
       </c>
     </row>
-    <row r="81" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>74</v>
       </c>
@@ -14942,7 +14960,7 @@
         <v>640.79554680614001</v>
       </c>
     </row>
-    <row r="82" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>75</v>
       </c>
@@ -15109,7 +15127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>76</v>
       </c>
@@ -15276,7 +15294,7 @@
         <v>26637.0946594546</v>
       </c>
     </row>
-    <row r="84" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>77</v>
       </c>
@@ -15443,7 +15461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>78</v>
       </c>
@@ -15610,7 +15628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>79</v>
       </c>
@@ -15777,7 +15795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>80</v>
       </c>
@@ -15944,7 +15962,7 @@
         <v>444358.77866852598</v>
       </c>
     </row>
-    <row r="88" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>81</v>
       </c>
@@ -16111,7 +16129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>82</v>
       </c>
@@ -16278,7 +16296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>83</v>
       </c>
@@ -16445,7 +16463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>84</v>
       </c>
@@ -16612,7 +16630,7 @@
         <v>134.36144478456001</v>
       </c>
     </row>
-    <row r="92" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>85</v>
       </c>
@@ -16779,7 +16797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>86</v>
       </c>
@@ -16946,7 +16964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>87</v>
       </c>
@@ -17113,7 +17131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>88</v>
       </c>
@@ -17280,7 +17298,7 @@
         <v>1870277.2868550201</v>
       </c>
     </row>
-    <row r="96" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>89</v>
       </c>
@@ -17447,7 +17465,7 @@
         <v>1633108.98250522</v>
       </c>
     </row>
-    <row r="97" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>90</v>
       </c>
@@ -17614,7 +17632,7 @@
         <v>2881.8506161075602</v>
       </c>
     </row>
-    <row r="98" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>91</v>
       </c>
@@ -17781,7 +17799,7 @@
         <v>6529060.0933931703</v>
       </c>
     </row>
-    <row r="99" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>92</v>
       </c>
@@ -17948,7 +17966,7 @@
         <v>62900.494945596198</v>
       </c>
     </row>
-    <row r="100" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>93</v>
       </c>
@@ -18115,7 +18133,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="101" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>94</v>
       </c>
@@ -18282,7 +18300,7 @@
         <v>889289.33473101899</v>
       </c>
     </row>
-    <row r="102" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>95</v>
       </c>
@@ -18449,7 +18467,7 @@
         <v>18162052.642346401</v>
       </c>
     </row>
-    <row r="103" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>96</v>
       </c>
@@ -18616,7 +18634,7 @@
         <v>281354.51899559598</v>
       </c>
     </row>
-    <row r="104" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>97</v>
       </c>
@@ -18783,7 +18801,7 @@
         <v>29120752.970029</v>
       </c>
     </row>
-    <row r="105" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>98</v>
       </c>
@@ -18950,7 +18968,7 @@
         <v>1396375.1864064999</v>
       </c>
     </row>
-    <row r="106" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>99</v>
       </c>
@@ -19117,7 +19135,7 @@
         <v>3055091.3636942599</v>
       </c>
     </row>
-    <row r="107" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>100</v>
       </c>
@@ -19284,7 +19302,7 @@
         <v>416393.37642184203</v>
       </c>
     </row>
-    <row r="108" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>101</v>
       </c>
@@ -19451,7 +19469,7 @@
         <v>3303.8599675713299</v>
       </c>
     </row>
-    <row r="109" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>102</v>
       </c>
@@ -19618,7 +19636,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>103</v>
       </c>
@@ -19785,7 +19803,7 @@
         <v>76875.520899697294</v>
       </c>
     </row>
-    <row r="111" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>104</v>
       </c>
@@ -19952,7 +19970,7 @@
         <v>838505.21722059394</v>
       </c>
     </row>
-    <row r="112" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>105</v>
       </c>
@@ -20119,7 +20137,7 @@
         <v>28500.821841189801</v>
       </c>
     </row>
-    <row r="113" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>106</v>
       </c>
@@ -20286,7 +20304,7 @@
         <v>180962.92509468301</v>
       </c>
     </row>
-    <row r="114" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>107</v>
       </c>
@@ -20453,7 +20471,7 @@
         <v>355997.382332996</v>
       </c>
     </row>
-    <row r="115" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>108</v>
       </c>
@@ -20620,7 +20638,7 @@
         <v>29519.680838538101</v>
       </c>
     </row>
-    <row r="116" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>109</v>
       </c>
@@ -20787,7 +20805,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="117" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>110</v>
       </c>
@@ -20954,7 +20972,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="118" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>111</v>
       </c>
@@ -21121,7 +21139,7 @@
         <v>1068498.6876640399</v>
       </c>
     </row>
-    <row r="119" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>112</v>
       </c>
@@ -21288,7 +21306,7 @@
         <v>3443795.3791314499</v>
       </c>
     </row>
-    <row r="120" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>113</v>
       </c>
@@ -21455,7 +21473,7 @@
         <v>1995673.06042319</v>
       </c>
     </row>
-    <row r="121" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>114</v>
       </c>
@@ -21622,7 +21640,7 @@
         <v>111878.72520518</v>
       </c>
     </row>
-    <row r="122" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>115</v>
       </c>
@@ -21789,7 +21807,7 @@
         <v>8381606.0462637497</v>
       </c>
     </row>
-    <row r="123" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>116</v>
       </c>
@@ -21956,7 +21974,7 @@
         <v>596146.38944250799</v>
       </c>
     </row>
-    <row r="124" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>117</v>
       </c>
@@ -22123,7 +22141,7 @@
         <v>7624.4236772609602</v>
       </c>
     </row>
-    <row r="125" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>118</v>
       </c>
@@ -22290,7 +22308,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="126" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>119</v>
       </c>
@@ -22457,7 +22475,7 @@
         <v>887954.53475918504</v>
       </c>
     </row>
-    <row r="127" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>120</v>
       </c>
@@ -22624,7 +22642,7 @@
         <v>267853.26513806102</v>
       </c>
     </row>
-    <row r="128" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>121</v>
       </c>
@@ -22791,7 +22809,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="129" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>122</v>
       </c>
@@ -22958,7 +22976,7 @@
         <v>23851.469615772701</v>
       </c>
     </row>
-    <row r="130" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>123</v>
       </c>
@@ -23125,7 +23143,7 @@
         <v>739863.40852495097</v>
       </c>
     </row>
-    <row r="131" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>124</v>
       </c>
@@ -23292,7 +23310,7 @@
         <v>271624.86485623399</v>
       </c>
     </row>
-    <row r="132" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>125</v>
       </c>
@@ -23459,7 +23477,7 @@
         <v>121339.50527135099</v>
       </c>
     </row>
-    <row r="133" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>126</v>
       </c>
@@ -23626,7 +23644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>127</v>
       </c>
@@ -23793,7 +23811,7 @@
         <v>1184055.9538423701</v>
       </c>
     </row>
-    <row r="135" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>128</v>
       </c>
@@ -23960,7 +23978,7 @@
         <v>458139.39371143101</v>
       </c>
     </row>
-    <row r="136" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>129</v>
       </c>
@@ -24127,7 +24145,7 @@
         <v>69436.715632198306</v>
       </c>
     </row>
-    <row r="137" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>130</v>
       </c>
@@ -24294,7 +24312,7 @@
         <v>314890.83522374899</v>
       </c>
     </row>
-    <row r="138" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>131</v>
       </c>
@@ -24461,7 +24479,7 @@
         <v>610849.947630323</v>
       </c>
     </row>
-    <row r="139" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>132</v>
       </c>
@@ -24628,7 +24646,7 @@
         <v>623296.63561608305</v>
       </c>
     </row>
-    <row r="140" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>133</v>
       </c>
@@ -24795,7 +24813,7 @@
         <v>74305.280662175704</v>
       </c>
     </row>
-    <row r="141" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>134</v>
       </c>
@@ -24962,7 +24980,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="142" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>135</v>
       </c>
@@ -25129,7 +25147,7 @@
         <v>54612.339208950398</v>
       </c>
     </row>
-    <row r="143" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>136</v>
       </c>
@@ -25296,7 +25314,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="144" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>137</v>
       </c>
@@ -25463,7 +25481,7 @@
         <v>349136.79658067401</v>
       </c>
     </row>
-    <row r="145" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>138</v>
       </c>
@@ -25630,7 +25648,7 @@
         <v>307879.19851238199</v>
       </c>
     </row>
-    <row r="146" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>139</v>
       </c>
@@ -25797,7 +25815,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="147" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>140</v>
       </c>
@@ -25964,7 +25982,7 @@
         <v>48081.280517557097</v>
       </c>
     </row>
-    <row r="148" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>141</v>
       </c>
@@ -26131,7 +26149,7 @@
         <v>72267.407837017396</v>
       </c>
     </row>
-    <row r="149" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>142</v>
       </c>
@@ -26298,7 +26316,7 @@
         <v>45705.773192368702</v>
       </c>
     </row>
-    <row r="150" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>143</v>
       </c>
@@ -26465,7 +26483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>144</v>
       </c>
@@ -26632,7 +26650,7 @@
         <v>109915.317895639</v>
       </c>
     </row>
-    <row r="152" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>145</v>
       </c>
@@ -26799,7 +26817,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="153" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>146</v>
       </c>
@@ -26966,7 +26984,7 @@
         <v>19538.072911703301</v>
       </c>
     </row>
-    <row r="154" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>147</v>
       </c>
@@ -27133,7 +27151,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="155" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>148</v>
       </c>
@@ -27300,7 +27318,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="156" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>149</v>
       </c>
@@ -27467,7 +27485,7 @@
         <v>125417.870714883</v>
       </c>
     </row>
-    <row r="157" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>150</v>
       </c>
@@ -27634,7 +27652,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="158" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>151</v>
       </c>
@@ -27801,7 +27819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>152</v>
       </c>
@@ -27968,7 +27986,7 @@
         <v>68969.529125264002</v>
       </c>
     </row>
-    <row r="160" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>153</v>
       </c>
@@ -28135,7 +28153,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="161" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>154</v>
       </c>
@@ -28302,7 +28320,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="162" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>155</v>
       </c>
@@ -28469,7 +28487,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="163" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>156</v>
       </c>
@@ -28636,7 +28654,7 @@
         <v>29591.463204604399</v>
       </c>
     </row>
-    <row r="164" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>157</v>
       </c>
@@ -28803,7 +28821,7 @@
         <v>65093.972967795497</v>
       </c>
     </row>
-    <row r="165" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>158</v>
       </c>
@@ -28970,7 +28988,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="166" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>159</v>
       </c>
@@ -29137,7 +29155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>160</v>
       </c>
@@ -29304,7 +29322,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="168" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>161</v>
       </c>
@@ -29471,7 +29489,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="169" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>162</v>
       </c>
@@ -29638,7 +29656,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="170" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>163</v>
       </c>
@@ -29805,7 +29823,7 @@
         <v>112834.187178971</v>
       </c>
     </row>
-    <row r="171" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>164</v>
       </c>
@@ -29972,7 +29990,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="172" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>165</v>
       </c>
@@ -30139,7 +30157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>166</v>
       </c>
@@ -30306,7 +30324,7 @@
         <v>317762.66817455</v>
       </c>
     </row>
-    <row r="174" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>167</v>
       </c>
@@ -30473,7 +30491,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="175" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>168</v>
       </c>
@@ -30640,7 +30658,7 @@
         <v>102814.168187156</v>
       </c>
     </row>
-    <row r="176" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>169</v>
       </c>
@@ -30807,7 +30825,7 @@
         <v>43099.511081577803</v>
       </c>
     </row>
-    <row r="177" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>170</v>
       </c>
@@ -30974,7 +30992,7 @@
         <v>36642.746691934</v>
       </c>
     </row>
-    <row r="178" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>171</v>
       </c>
@@ -31141,7 +31159,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="179" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>172</v>
       </c>
@@ -31308,7 +31326,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="180" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>173</v>
       </c>
@@ -31475,7 +31493,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="181" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>174</v>
       </c>
@@ -31642,7 +31660,7 @@
         <v>29866.484965920499</v>
       </c>
     </row>
-    <row r="182" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>175</v>
       </c>
@@ -31809,7 +31827,7 @@
         <v>492349.33677530597</v>
       </c>
     </row>
-    <row r="183" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>176</v>
       </c>
@@ -31976,7 +31994,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="184" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>177</v>
       </c>
@@ -32143,7 +32161,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="185" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>178</v>
       </c>
@@ -32310,7 +32328,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="186" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>179</v>
       </c>
@@ -32477,7 +32495,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="187" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>180</v>
       </c>
@@ -32644,7 +32662,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="188" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>181</v>
       </c>
@@ -32811,7 +32829,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="189" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>182</v>
       </c>
@@ -32978,7 +32996,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="190" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>183</v>
       </c>
@@ -33145,7 +33163,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="191" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>184</v>
       </c>
@@ -33312,7 +33330,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="192" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>185</v>
       </c>
@@ -33479,7 +33497,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="193" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>186</v>
       </c>
@@ -33646,7 +33664,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="194" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>187</v>
       </c>
@@ -33813,7 +33831,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="195" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>188</v>
       </c>
@@ -33980,7 +33998,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="196" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>189</v>
       </c>
@@ -34147,7 +34165,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="197" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>190</v>
       </c>
@@ -34314,7 +34332,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="198" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>191</v>
       </c>
@@ -34481,7 +34499,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="199" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>192</v>
       </c>
@@ -34649,8 +34667,392 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:BC7"/>
+  <autoFilter ref="A7:BC199">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="SADC"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BC9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:55" s="6" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z1" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG1" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH1" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AO1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AP1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AT1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AU1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="AV1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AW1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="AX1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AY1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AZ1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="BA1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="BC1" s="25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:55" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="45">
+        <v>45</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="46">
+        <v>50491000</v>
+      </c>
+      <c r="G2" s="45">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="H2" s="45">
+        <v>1</v>
+      </c>
+      <c r="I2" s="47">
+        <v>0.63</v>
+      </c>
+      <c r="J2" s="48">
+        <v>0.11104648637144</v>
+      </c>
+      <c r="K2" s="48">
+        <v>0.990670370448134</v>
+      </c>
+      <c r="L2" s="45">
+        <v>423.0129</v>
+      </c>
+      <c r="M2" s="46">
+        <v>42.042681338324499</v>
+      </c>
+      <c r="N2" s="49">
+        <v>8.3267674116821802E-2</v>
+      </c>
+      <c r="O2" s="46">
+        <v>23717.690929909499</v>
+      </c>
+      <c r="P2" s="46">
+        <v>211590.788934235</v>
+      </c>
+      <c r="Q2" s="46">
+        <v>4464.3185953444799</v>
+      </c>
+      <c r="R2" s="46">
+        <v>2625.5469586024401</v>
+      </c>
+      <c r="S2" s="46">
+        <v>1015.91760704213</v>
+      </c>
+      <c r="T2" s="46">
+        <v>1251.8698806069301</v>
+      </c>
+      <c r="U2" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="V2" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="W2" s="50">
+        <v>3756.4611377111701</v>
+      </c>
+      <c r="X2" s="50">
+        <v>2625.5469586024401</v>
+      </c>
+      <c r="Y2" s="50">
+        <v>1015.91760704213</v>
+      </c>
+      <c r="Z2" s="46">
+        <v>26827764.6526573</v>
+      </c>
+      <c r="AA2" s="46">
+        <v>1475505.31449352</v>
+      </c>
+      <c r="AB2" s="46">
+        <v>16597531.623279501</v>
+      </c>
+      <c r="AC2" s="46">
+        <v>18793142.645831499</v>
+      </c>
+      <c r="AD2" s="46">
+        <v>2880000.0155807999</v>
+      </c>
+      <c r="AE2" s="46">
+        <v>200033.518764087</v>
+      </c>
+      <c r="AF2" s="46">
+        <v>2436.2484925111298</v>
+      </c>
+      <c r="AG2" s="46">
+        <v>37599.961022399999</v>
+      </c>
+      <c r="AH2" s="46">
+        <v>8.2957201696978107</v>
+      </c>
+      <c r="AI2" s="46">
+        <v>64.950596441323796</v>
+      </c>
+      <c r="AJ2" s="46">
+        <v>5030.5087591435004</v>
+      </c>
+      <c r="AK2" s="46">
+        <v>27745.848510358999</v>
+      </c>
+      <c r="AL2" s="46">
+        <v>48371.338742515298</v>
+      </c>
+      <c r="AM2" s="46">
+        <v>220129.11446685399</v>
+      </c>
+      <c r="AN2" s="46">
+        <v>992.03393350106103</v>
+      </c>
+      <c r="AO2" s="46">
+        <v>5981.4500763463802</v>
+      </c>
+      <c r="AP2" s="46">
+        <v>493.13645038112702</v>
+      </c>
+      <c r="AQ2" s="46">
+        <v>4094.5841376123099</v>
+      </c>
+      <c r="AR2" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS2" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT2" s="46">
+        <v>5967372.2782135103</v>
+      </c>
+      <c r="AU2" s="46">
+        <v>28141369.782428101</v>
+      </c>
+      <c r="AV2" s="46">
+        <v>283500.52408952301</v>
+      </c>
+      <c r="AW2" s="46">
+        <v>1268262.8107654401</v>
+      </c>
+      <c r="AX2" s="46">
+        <v>3722553.9967495799</v>
+      </c>
+      <c r="AY2" s="46">
+        <v>17526916.647193499</v>
+      </c>
+      <c r="AZ2" s="46">
+        <v>3770648.3309994601</v>
+      </c>
+      <c r="BA2" s="46">
+        <v>29072842.423985299</v>
+      </c>
+      <c r="BB2" s="46">
+        <v>158.62916825760101</v>
+      </c>
+      <c r="BC2" s="46">
+        <v>77310.888517116298</v>
+      </c>
+    </row>
+    <row r="8" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>471</v>
+      </c>
+      <c r="B8" t="s">
+        <v>472</v>
+      </c>
+      <c r="C8" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="9" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f>L2 * F2/100000</f>
+        <v>213583.44333900002</v>
+      </c>
+      <c r="B9">
+        <f>J2*A9</f>
+        <v>23717.690929909495</v>
+      </c>
+      <c r="C9">
+        <f>A9-B9</f>
+        <v>189865.75240909052</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>